<commit_message>
Adding content to the readme file
</commit_message>
<xml_diff>
--- a/OWASP_Test_Guide_V4_In_Practice/Reporting/OWASP_Test_Guide_v4.xlsx
+++ b/OWASP_Test_Guide_V4_In_Practice/Reporting/OWASP_Test_Guide_v4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="10800" windowWidth="40220" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27740" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="107">
   <si>
     <t>I Information Gathering</t>
   </si>
@@ -322,15 +322,6 @@
     <t>Testing for default credentials (OTG-AUTHN-002)</t>
   </si>
   <si>
-    <t>Objective</t>
-  </si>
-  <si>
-    <t>Tools</t>
-  </si>
-  <si>
-    <t>Instructions</t>
-  </si>
-  <si>
     <t>QA Involvement</t>
   </si>
   <si>
@@ -338,16 +329,44 @@
   </si>
   <si>
     <t>Dev Involvement</t>
+  </si>
+  <si>
+    <t>Open Source Tools</t>
+  </si>
+  <si>
+    <t>Commercial Tools</t>
+  </si>
+  <si>
+    <t>curl, nmap, openssl,sslyze</t>
+  </si>
+  <si>
+    <t>Sites</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,13 +389,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -709,13 +738,17 @@
   <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
@@ -725,33 +758,33 @@
       <c r="A1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="F1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:8" ht="45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -759,31 +792,31 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="30">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -791,23 +824,23 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="30">
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="30">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -815,7 +848,7 @@
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -823,47 +856,47 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="30">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="30">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="30">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="30">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="30">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>96</v>
       </c>
     </row>
@@ -871,15 +904,15 @@
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="30">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -887,7 +920,7 @@
       <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -895,7 +928,7 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -903,39 +936,39 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="30">
       <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="30">
       <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="30">
       <c r="A24" t="s">
         <v>18</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" ht="30">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -943,87 +976,87 @@
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" ht="30">
       <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" ht="30">
       <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" ht="30">
       <c r="A29" t="s">
         <v>24</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" ht="30">
       <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" ht="30">
       <c r="A31" t="s">
         <v>24</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" ht="30">
       <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" ht="30">
       <c r="A33" t="s">
         <v>24</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" ht="30">
       <c r="A34" t="s">
         <v>24</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" ht="30">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" ht="30">
       <c r="A36" t="s">
         <v>33</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1031,23 +1064,23 @@
       <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" ht="30">
       <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" ht="30">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1055,7 +1088,7 @@
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1063,23 +1096,23 @@
       <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" ht="30">
       <c r="A42" t="s">
         <v>38</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" ht="30">
       <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1087,7 +1120,7 @@
       <c r="A44" t="s">
         <v>38</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1095,7 +1128,7 @@
       <c r="A45" t="s">
         <v>38</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1103,39 +1136,39 @@
       <c r="A46" t="s">
         <v>38</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" ht="30">
       <c r="A47" t="s">
         <v>47</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" ht="30">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" ht="30">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" ht="30">
       <c r="A50" t="s">
         <v>47</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1143,7 +1176,7 @@
       <c r="A51" t="s">
         <v>47</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1151,7 +1184,7 @@
       <c r="A52" t="s">
         <v>47</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1159,7 +1192,7 @@
       <c r="A53" t="s">
         <v>47</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1167,7 +1200,7 @@
       <c r="A54" t="s">
         <v>47</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1175,7 +1208,7 @@
       <c r="A55" t="s">
         <v>47</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1183,7 +1216,7 @@
       <c r="A56" t="s">
         <v>47</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1191,7 +1224,7 @@
       <c r="A57" t="s">
         <v>47</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1199,15 +1232,15 @@
       <c r="A58" t="s">
         <v>47</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" ht="30">
       <c r="A59" t="s">
         <v>47</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1215,23 +1248,23 @@
       <c r="A60" t="s">
         <v>47</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" ht="30">
       <c r="A61" t="s">
         <v>47</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" ht="30">
       <c r="A62" t="s">
         <v>47</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1239,7 +1272,7 @@
       <c r="A63" t="s">
         <v>64</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1247,135 +1280,138 @@
       <c r="A64" t="s">
         <v>64</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:3" ht="30">
       <c r="A65" t="s">
         <v>67</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:3" ht="30">
       <c r="A67" t="s">
         <v>67</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:3" ht="30">
       <c r="A68" t="s">
         <v>79</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:3" ht="30">
       <c r="A69" t="s">
         <v>79</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>79</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>79</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:3" ht="30">
       <c r="A72" t="s">
         <v>79</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:3" ht="30">
       <c r="A73" t="s">
         <v>79</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:3" ht="30">
       <c r="A74" t="s">
         <v>79</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:3" ht="30">
       <c r="A75" t="s">
         <v>79</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:3" ht="30">
       <c r="A76" t="s">
         <v>79</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:3" ht="30">
       <c r="A77" t="s">
         <v>83</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:3" ht="30">
       <c r="A78" t="s">
         <v>83</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>83</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:3" ht="30">
       <c r="A80" t="s">
         <v>83</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1383,23 +1419,23 @@
       <c r="A81" t="s">
         <v>83</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" ht="30">
       <c r="A82" t="s">
         <v>83</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" ht="30">
       <c r="A83" t="s">
         <v>83</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1407,7 +1443,7 @@
       <c r="A84" t="s">
         <v>83</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1415,7 +1451,7 @@
       <c r="A85" t="s">
         <v>83</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1423,7 +1459,7 @@
       <c r="A86" t="s">
         <v>83</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1431,7 +1467,7 @@
       <c r="A87" t="s">
         <v>83</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1439,12 +1475,13 @@
       <c r="A88" t="s">
         <v>83</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>